<commit_message>
Auto scrolling and darkening of past events complete
</commit_message>
<xml_diff>
--- a/Mission Times.xlsx
+++ b/Mission Times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Java\Current Projects\Apollo 11 Anniversary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A96FBA-9112-4146-B20D-DDD94021AB5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D98A9A7-AC4B-4E9B-946F-61E379EB8C80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23415" windowHeight="3405" xr2:uid="{E2A0F91F-357B-4B6D-B279-70CDC83B58C3}"/>
   </bookViews>
@@ -1482,8 +1482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC65548-14F0-4955-8FE0-2180CBE49E18}">
   <dimension ref="A1:D248"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A155" sqref="A155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>